<commit_message>
Nouveau lien de la RP Cinezone et mise à jour du tabeau de synthèse
</commit_message>
<xml_diff>
--- a/image_logo/Tableau de synthèse - Epreuve E4 - BTS SIO - EXCEL.xlsx
+++ b/image_logo/Tableau de synthèse - Epreuve E4 - BTS SIO - EXCEL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nedjb\Documents\PROJET IT\PORTFOLIO\image_logo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2046A0F8-4015-4294-BBB2-922AEF4F3B98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE3604DA-A8D5-4D59-9F1E-58B2E6DCEFC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5364" yWindow="336" windowWidth="17280" windowHeight="11448" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tableau de synthèse Épreuve E4" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="39">
   <si>
     <t>BTS SERVICES INFORMATIQUES AUX ORGANISATIONS</t>
   </si>
@@ -176,6 +176,18 @@
   </si>
   <si>
     <t>Adresse URL du portfolio : https://delcoco95.github.io/mon-portfolio/</t>
+  </si>
+  <si>
+    <t>14/05 au 25/05/2025</t>
+  </si>
+  <si>
+    <t>14/05 au 25/05/2026</t>
+  </si>
+  <si>
+    <t>13/05 au 28/05/2027</t>
+  </si>
+  <si>
+    <t>25/05 au 20/07/2025</t>
   </si>
 </sst>
 </file>
@@ -715,15 +727,39 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -755,30 +791,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1091,8 +1103,8 @@
   </sheetPr>
   <dimension ref="A1:AQ81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:H5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1105,56 +1117,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25" t="s">
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="25"/>
+      <c r="H1" s="23"/>
     </row>
     <row r="2" spans="1:43" ht="41.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
     </row>
     <row r="3" spans="1:43" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="43" t="s">
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="38"/>
-      <c r="H3" s="44"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="31"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="42"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="29"/>
       <c r="F4" s="12" t="s">
         <v>4</v>
       </c>
@@ -1166,22 +1178,22 @@
       </c>
     </row>
     <row r="5" spans="1:43" ht="39.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="36"/>
+      <c r="B5" s="43"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="44"/>
     </row>
     <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="40" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -1204,8 +1216,8 @@
       </c>
     </row>
     <row r="7" spans="1:43" s="2" customFormat="1" ht="324.89999999999998" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="24"/>
-      <c r="B7" s="33"/>
+      <c r="A7" s="33"/>
+      <c r="B7" s="41"/>
       <c r="C7" s="20" t="s">
         <v>14</v>
       </c>
@@ -1261,16 +1273,16 @@
       <c r="AQ7"/>
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="28"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="36"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1311,8 +1323,8 @@
       <c r="A9" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="22">
-        <v>2025</v>
+      <c r="B9" s="22" t="s">
+        <v>35</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>26</v>
@@ -1370,8 +1382,8 @@
       <c r="A10" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="22">
-        <v>2025</v>
+      <c r="B10" s="22" t="s">
+        <v>36</v>
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="14" t="s">
@@ -1425,8 +1437,8 @@
       <c r="A11" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="22">
-        <v>2025</v>
+      <c r="B11" s="22" t="s">
+        <v>37</v>
       </c>
       <c r="C11" s="15"/>
       <c r="D11" s="14" t="s">
@@ -1480,8 +1492,8 @@
       <c r="A12" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="22">
-        <v>2025</v>
+      <c r="B12" s="22" t="s">
+        <v>38</v>
       </c>
       <c r="C12" s="15"/>
       <c r="D12" s="15"/>
@@ -1816,16 +1828,16 @@
       <c r="AQ18"/>
     </row>
     <row r="19" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A19" s="29" t="s">
+      <c r="A19" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="30"/>
-      <c r="C19" s="30"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="30"/>
-      <c r="F19" s="30"/>
-      <c r="G19" s="30"/>
-      <c r="H19" s="31"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="39"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -2178,16 +2190,16 @@
       <c r="AQ26"/>
     </row>
     <row r="27" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A27" s="29" t="s">
+      <c r="A27" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="B27" s="30"/>
-      <c r="C27" s="30"/>
-      <c r="D27" s="30"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="30"/>
-      <c r="G27" s="30"/>
-      <c r="H27" s="31"/>
+      <c r="B27" s="38"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="39"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -2632,11 +2644,6 @@
     <row r="81" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F3:H3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A8:H8"/>
@@ -2644,6 +2651,11 @@
     <mergeCell ref="A27:H27"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A5:H5"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -2654,15 +2666,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="665588ff-5dd3-431a-aaf4-bd4a76d54561">
@@ -2671,6 +2674,15 @@
     <TaxCatchAll xmlns="8dfcfa40-b15b-4f0f-a13d-24527312d446" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2875,14 +2887,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A9CD917-9C6C-4808-B3EB-08BF761FD3DB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B48EC0E1-0992-4BEA-AB73-03077E430CDC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -2895,6 +2899,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="8dfcfa40-b15b-4f0f-a13d-24527312d446"/>
     <ds:schemaRef ds:uri="665588ff-5dd3-431a-aaf4-bd4a76d54561"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A9CD917-9C6C-4808-B3EB-08BF761FD3DB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>